<commit_message>
Ajout de la correction du sprint 2
</commit_message>
<xml_diff>
--- a/Equipe101.xlsx
+++ b/Equipe101.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="8_{A9B08717-0A78-4896-A8AA-F48CA0C7A758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0768827-B422-422F-8EA7-122460B894F0}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="8_{A9B08717-0A78-4896-A8AA-F48CA0C7A758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AF6B876-3413-4BA0-9CF3-B7172E1096C0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="9" r:id="rId1"/>
@@ -26,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="164">
   <si>
     <t>Fonct.</t>
   </si>
@@ -154,6 +155,11 @@
 Les ViewChild() peuven être privés</t>
   </si>
   <si>
+    <t xml:space="preserve"> Quand les attributs ne sont utilisés que dans une classe, ils doivent être privés
+Les ViewChild() peuven être privés
+Exemple dans : GamePreparationPageComponent</t>
+  </si>
+  <si>
     <t>2.5 Valeur par défaut</t>
   </si>
   <si>
@@ -163,6 +169,10 @@
     <t>sidebar.component.ts : countdown initialisé differemment
 waiting-room.component.ts : gameStarted initialisé differemment
 Pareil dans GameJoinPageComponent, GamePreparationPageComponent, etc ...</t>
+  </si>
+  <si>
+    <t>Vos Input() et @Output() sont initialisés différemment
+LeaderboardPageComponent.displayedColumns initialisé différemment</t>
   </si>
   <si>
     <t>3. Fonctions</t>
@@ -278,6 +288,9 @@
     <t>l104 dans player.service + l220 du server/room.ts utilisez des variables booleennes</t>
   </si>
   <si>
+    <t>L143 et L147 de  client/src/app/services/key-manager.service.ts L44 de server/app/classes/game/board.ts L103 et L172 de server/app/classes/game/game.ts : veuillez utiliser des variables booleenes pour simplifier les predicats</t>
+  </si>
+  <si>
     <t>7. Qualité générale</t>
   </si>
   <si>
@@ -315,6 +328,9 @@
     <t>Le code n'utilise pas d'objets anonymes JS et priorise les classes et les interfaces.</t>
   </si>
   <si>
+    <t>les fichiers *Effects ont une action de type any, implicit</t>
+  </si>
+  <si>
     <t>7.5 Duplication</t>
   </si>
   <si>
@@ -331,6 +347,9 @@
     <t>Eslint disable sans justification</t>
   </si>
   <si>
+    <t>eslint-disable no-invalid-this pour des fichiers entiers? ; eslint-disable-next-line @typescript-eslint/prefer-for-of (Si vous n'utilisez ni l'index ni l'élément du tableau, un while)</t>
+  </si>
+  <si>
     <t>7.7 Imbrication</t>
   </si>
   <si>
@@ -338,6 +357,9 @@
   </si>
   <si>
     <t>Pas toujours utilisé (Bon effort!)</t>
+  </si>
+  <si>
+    <t>Pas toujours utilisé</t>
   </si>
   <si>
     <t>7.8 Performance</t>
@@ -468,6 +490,9 @@
     <t>2.3 Meilleurs scores</t>
   </si>
   <si>
+    <t>Le système doit afficher un tableau pour le mode classique et le mode LOG2990_ dans une modale.</t>
+  </si>
+  <si>
     <t>2.4 Paramètres de partie - minuterie</t>
   </si>
   <si>
@@ -483,10 +508,16 @@
     <t>2.8 Commande réserve</t>
   </si>
   <si>
+    <t>Les lettre de la reserve inclus les lettre du chevalet du JV</t>
+  </si>
+  <si>
     <t>2.9 Manipuler les lettres du chevalet</t>
   </si>
   <si>
     <t>2.10 Commande indice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le client fait des connections reeles au socket server !! erreur de console sur le navigateur quand on lance les tests du client par rapport a la connexion refusee sur les sockets. </t>
   </si>
   <si>
     <t>Erreur de build  / déploiement erroné</t>
@@ -2146,29 +2177,98 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2209,74 +2309,14 @@
     <xf numFmtId="9" fontId="13" fillId="10" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2310,15 +2350,6 @@
     </xf>
     <xf numFmtId="2" fontId="17" fillId="20" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2712,7 +2743,7 @@
   <dimension ref="A3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2777,15 +2808,15 @@
       </c>
       <c r="B5" s="113">
         <f>(Fonctionnalités!E34)</f>
-        <v>0</v>
+        <v>0.96700000000000008</v>
       </c>
       <c r="C5" s="113">
         <f>'Assurance Qualité'!F60</f>
-        <v>0</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="D5" s="113">
         <f t="shared" ref="D5:D6" si="0">B5*0.6+C5*0.4 - 0.1*E5</f>
-        <v>0</v>
+        <v>0.92220000000000013</v>
       </c>
       <c r="E5" s="114"/>
       <c r="F5" s="115">
@@ -2793,7 +2824,7 @@
       </c>
       <c r="G5" s="116">
         <f t="shared" ref="G5:G7" si="1">D5*F5</f>
-        <v>0</v>
+        <v>23.055000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2849,8 +2880,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:Q60"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2869,36 +2900,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A2" s="258" t="s">
+      <c r="A2" s="225" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="258"/>
-      <c r="C2" s="258"/>
-      <c r="D2" s="258"/>
-      <c r="E2" s="258"/>
-      <c r="F2" s="258"/>
-      <c r="G2" s="258"/>
-      <c r="H2" s="258"/>
-      <c r="I2" s="258"/>
-      <c r="J2" s="258"/>
-      <c r="K2" s="258"/>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="225"/>
+      <c r="K2" s="225"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
     <row r="4" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A4" s="259" t="s">
+      <c r="A4" s="226" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="259"/>
-      <c r="C4" s="259"/>
-      <c r="D4" s="259"/>
-      <c r="E4" s="259"/>
-      <c r="F4" s="259"/>
-      <c r="G4" s="259"/>
-      <c r="H4" s="259"/>
-      <c r="I4" s="259"/>
-      <c r="J4" s="259"/>
-      <c r="K4" s="259"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
@@ -2921,7 +2952,7 @@
       <c r="A6" s="246" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="263" t="s">
+      <c r="B6" s="230" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="248" t="s">
@@ -2934,11 +2965,11 @@
       </c>
       <c r="G6" s="251"/>
       <c r="H6" s="252"/>
-      <c r="I6" s="260" t="s">
+      <c r="I6" s="227" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="261"/>
-      <c r="K6" s="262"/>
+      <c r="J6" s="228"/>
+      <c r="K6" s="229"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="244"/>
@@ -2947,7 +2978,7 @@
     </row>
     <row r="7" spans="1:17" ht="18.75">
       <c r="A7" s="247"/>
-      <c r="B7" s="264"/>
+      <c r="B7" s="231"/>
       <c r="C7" s="14" t="s">
         <v>14</v>
       </c>
@@ -2983,26 +3014,28 @@
       <c r="Q7" s="40"/>
     </row>
     <row r="8" spans="1:17" ht="18.75">
-      <c r="A8" s="229" t="s">
+      <c r="A8" s="243" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="229"/>
-      <c r="C8" s="227" t="s">
+      <c r="B8" s="243"/>
+      <c r="C8" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="228"/>
+      <c r="D8" s="233"/>
       <c r="E8" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="227" t="s">
+      <c r="F8" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="228"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="227" t="s">
+      <c r="G8" s="233"/>
+      <c r="H8" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="228"/>
+      <c r="J8" s="233"/>
       <c r="K8" s="46"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -3011,7 +3044,7 @@
       <c r="P8" s="40"/>
       <c r="Q8" s="40"/>
     </row>
-    <row r="9" spans="1:17" ht="60">
+    <row r="9" spans="1:17" ht="60.75">
       <c r="A9" s="29" t="s">
         <v>19</v>
       </c>
@@ -3027,7 +3060,9 @@
       <c r="E9" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="102"/>
+      <c r="F9" s="102">
+        <v>1</v>
+      </c>
       <c r="G9" s="99">
         <v>6</v>
       </c>
@@ -3044,7 +3079,7 @@
       <c r="P9" s="40"/>
       <c r="Q9" s="40"/>
     </row>
-    <row r="10" spans="1:17" ht="45">
+    <row r="10" spans="1:17" ht="45.75">
       <c r="A10" s="23" t="s">
         <v>22</v>
       </c>
@@ -3060,7 +3095,9 @@
       <c r="E10" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="102"/>
+      <c r="F10" s="102">
+        <v>1</v>
+      </c>
       <c r="G10" s="99">
         <v>2</v>
       </c>
@@ -3078,10 +3115,10 @@
       <c r="Q10" s="40"/>
     </row>
     <row r="11" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A11" s="222" t="s">
+      <c r="A11" s="236" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="223"/>
+      <c r="B11" s="237"/>
       <c r="C11" s="47">
         <f>SUMPRODUCT(C6:C10,D6:D10)</f>
         <v>6.4</v>
@@ -3093,7 +3130,7 @@
       <c r="E11" s="49"/>
       <c r="F11" s="50">
         <f>SUMPRODUCT(F6:F10,G6:G10)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G11" s="51">
         <f>SUM(G6:G10)</f>
@@ -3117,26 +3154,28 @@
       <c r="Q11" s="44"/>
     </row>
     <row r="12" spans="1:17" s="12" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A12" s="229" t="s">
+      <c r="A12" s="243" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="229"/>
-      <c r="C12" s="227" t="s">
+      <c r="B12" s="243"/>
+      <c r="C12" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="228"/>
+      <c r="D12" s="233"/>
       <c r="E12" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="227" t="s">
+      <c r="F12" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="228"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="227" t="s">
+      <c r="G12" s="233"/>
+      <c r="H12" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="228"/>
+      <c r="J12" s="233"/>
       <c r="K12" s="46"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -3145,7 +3184,7 @@
       <c r="P12" s="43"/>
       <c r="Q12" s="43"/>
     </row>
-    <row r="13" spans="1:17" ht="30">
+    <row r="13" spans="1:17" ht="30.75">
       <c r="A13" s="29" t="s">
         <v>27</v>
       </c>
@@ -3159,7 +3198,9 @@
         <v>4</v>
       </c>
       <c r="E13" s="81"/>
-      <c r="F13" s="89"/>
+      <c r="F13" s="89">
+        <v>1</v>
+      </c>
       <c r="G13" s="90">
         <v>4</v>
       </c>
@@ -3172,7 +3213,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="30">
+    <row r="14" spans="1:17" ht="30.75">
       <c r="A14" s="23" t="s">
         <v>29</v>
       </c>
@@ -3186,7 +3227,9 @@
         <v>2</v>
       </c>
       <c r="E14" s="85"/>
-      <c r="F14" s="86"/>
+      <c r="F14" s="86">
+        <v>1</v>
+      </c>
       <c r="G14" s="87">
         <v>2</v>
       </c>
@@ -3199,7 +3242,7 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:17" ht="45">
+    <row r="15" spans="1:17" ht="45.75">
       <c r="A15" s="23" t="s">
         <v>31</v>
       </c>
@@ -3213,7 +3256,9 @@
         <v>3</v>
       </c>
       <c r="E15" s="85"/>
-      <c r="F15" s="86"/>
+      <c r="F15" s="86">
+        <v>1</v>
+      </c>
       <c r="G15" s="87">
         <v>3</v>
       </c>
@@ -3226,7 +3271,7 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="90">
+    <row r="16" spans="1:17" ht="137.25">
       <c r="A16" s="23" t="s">
         <v>33</v>
       </c>
@@ -3242,11 +3287,15 @@
       <c r="E16" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="86"/>
+      <c r="F16" s="86">
+        <v>0</v>
+      </c>
       <c r="G16" s="87">
         <v>2</v>
       </c>
-      <c r="H16" s="88"/>
+      <c r="H16" s="88" t="s">
+        <v>36</v>
+      </c>
       <c r="I16" s="76"/>
       <c r="J16" s="77">
         <v>2</v>
@@ -3255,12 +3304,12 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:17" ht="225">
+    <row r="17" spans="1:17" ht="183">
       <c r="A17" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" s="83">
         <v>0</v>
@@ -3269,13 +3318,17 @@
         <v>4</v>
       </c>
       <c r="E17" s="85" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="86"/>
+        <v>39</v>
+      </c>
+      <c r="F17" s="86">
+        <v>0.5</v>
+      </c>
       <c r="G17" s="87">
         <v>4</v>
       </c>
-      <c r="H17" s="88"/>
+      <c r="H17" s="88" t="s">
+        <v>40</v>
+      </c>
       <c r="I17" s="76"/>
       <c r="J17" s="77">
         <v>4</v>
@@ -3285,10 +3338,10 @@
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A18" s="222" t="s">
+      <c r="A18" s="236" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="223"/>
+      <c r="B18" s="237"/>
       <c r="C18" s="47">
         <f>SUMPRODUCT(C13:C17,D13:D17)</f>
         <v>9</v>
@@ -3300,7 +3353,7 @@
       <c r="E18" s="49"/>
       <c r="F18" s="50">
         <f>SUMPRODUCT(F13:F17,G13:G17)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G18" s="51">
         <f>SUM(G13:G17)</f>
@@ -3324,36 +3377,38 @@
       <c r="Q18" s="44"/>
     </row>
     <row r="19" spans="1:17" s="43" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A19" s="243" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="243"/>
-      <c r="C19" s="227" t="s">
+      <c r="A19" s="242" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="242"/>
+      <c r="C19" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="228"/>
+      <c r="D19" s="233"/>
       <c r="E19" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="227" t="s">
+      <c r="F19" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="228"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="227" t="s">
+      <c r="G19" s="233"/>
+      <c r="H19" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="228"/>
+      <c r="J19" s="233"/>
       <c r="K19" s="46"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:17" ht="30">
+    <row r="20" spans="1:17" ht="30.75">
       <c r="A20" s="29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20" s="97">
         <v>1</v>
@@ -3362,7 +3417,9 @@
         <v>2</v>
       </c>
       <c r="E20" s="26"/>
-      <c r="F20" s="82"/>
+      <c r="F20" s="82">
+        <v>1</v>
+      </c>
       <c r="G20" s="27">
         <v>2</v>
       </c>
@@ -3375,12 +3432,12 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="1:17" ht="120">
+    <row r="21" spans="1:17" ht="106.5">
       <c r="A21" s="23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" s="83">
         <v>0.75</v>
@@ -3389,9 +3446,11 @@
         <v>3</v>
       </c>
       <c r="E21" s="85" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="86"/>
+        <v>46</v>
+      </c>
+      <c r="F21" s="86">
+        <v>1</v>
+      </c>
       <c r="G21" s="87">
         <v>3</v>
       </c>
@@ -3404,12 +3463,12 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="1:17" ht="30">
+    <row r="22" spans="1:17" ht="30.75">
       <c r="A22" s="23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C22" s="83">
         <v>1</v>
@@ -3418,7 +3477,9 @@
         <v>3</v>
       </c>
       <c r="E22" s="85"/>
-      <c r="F22" s="86"/>
+      <c r="F22" s="86">
+        <v>1</v>
+      </c>
       <c r="G22" s="87">
         <v>3</v>
       </c>
@@ -3432,10 +3493,10 @@
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A23" s="265" t="s">
+      <c r="A23" s="234" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="254"/>
+      <c r="B23" s="235"/>
       <c r="C23" s="57">
         <f>SUMPRODUCT(C20:C22,D20:D22)</f>
         <v>7.25</v>
@@ -3447,7 +3508,7 @@
       <c r="E23" s="59"/>
       <c r="F23" s="60">
         <f>SUMPRODUCT(F20:F22,G20:G22)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G23" s="61">
         <f>SUM(G20:G22)</f>
@@ -3468,35 +3529,37 @@
     </row>
     <row r="24" spans="1:17" ht="18.75" customHeight="1">
       <c r="A24" s="45" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B24" s="45"/>
-      <c r="C24" s="227" t="s">
+      <c r="C24" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="228"/>
+      <c r="D24" s="233"/>
       <c r="E24" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="227" t="s">
+      <c r="F24" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="228"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="227" t="s">
+      <c r="G24" s="233"/>
+      <c r="H24" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="228"/>
+      <c r="J24" s="233"/>
       <c r="K24" s="46"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="1:17" ht="30">
+    <row r="25" spans="1:17" ht="30.75">
       <c r="A25" s="42" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C25" s="97">
         <v>0</v>
@@ -3504,10 +3567,12 @@
       <c r="D25" s="25">
         <v>2</v>
       </c>
-      <c r="E25" s="255" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="82"/>
+      <c r="E25" s="239" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="82">
+        <v>1</v>
+      </c>
       <c r="G25" s="27">
         <v>2</v>
       </c>
@@ -3522,10 +3587,10 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C26" s="83">
         <v>0</v>
@@ -3533,8 +3598,10 @@
       <c r="D26" s="84">
         <v>1</v>
       </c>
-      <c r="E26" s="256"/>
-      <c r="F26" s="86"/>
+      <c r="E26" s="240"/>
+      <c r="F26" s="86">
+        <v>1</v>
+      </c>
       <c r="G26" s="87">
         <v>1</v>
       </c>
@@ -3549,10 +3616,10 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C27" s="83">
         <v>0</v>
@@ -3560,8 +3627,10 @@
       <c r="D27" s="84">
         <v>1</v>
       </c>
-      <c r="E27" s="257"/>
-      <c r="F27" s="86"/>
+      <c r="E27" s="241"/>
+      <c r="F27" s="86">
+        <v>1</v>
+      </c>
       <c r="G27" s="87">
         <v>1</v>
       </c>
@@ -3575,10 +3644,10 @@
       <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A28" s="253" t="s">
+      <c r="A28" s="238" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="254"/>
+      <c r="B28" s="235"/>
       <c r="C28" s="47">
         <f>SUMPRODUCT(C25:C27,D25:D27)</f>
         <v>0</v>
@@ -3590,7 +3659,7 @@
       <c r="E28" s="49"/>
       <c r="F28" s="60">
         <f>SUMPRODUCT(F25:F27,G25:G27)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G28" s="61">
         <f>SUM(G25:G27)</f>
@@ -3610,34 +3679,34 @@
       <c r="M28" s="56"/>
     </row>
     <row r="29" spans="1:17" ht="21" customHeight="1">
-      <c r="A29" s="243" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="243"/>
-      <c r="C29" s="227" t="s">
+      <c r="A29" s="242" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="242"/>
+      <c r="C29" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="228"/>
+      <c r="D29" s="233"/>
       <c r="E29" s="46"/>
-      <c r="F29" s="227" t="s">
+      <c r="F29" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="228"/>
+      <c r="G29" s="233"/>
       <c r="H29" s="66"/>
-      <c r="I29" s="227" t="s">
+      <c r="I29" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="J29" s="228"/>
+      <c r="J29" s="233"/>
       <c r="K29" s="46"/>
       <c r="L29" s="9"/>
       <c r="M29" s="4"/>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="31" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C30" s="79">
         <v>1</v>
@@ -3646,7 +3715,9 @@
         <v>2</v>
       </c>
       <c r="E30" s="81"/>
-      <c r="F30" s="89"/>
+      <c r="F30" s="89">
+        <v>1</v>
+      </c>
       <c r="G30" s="90">
         <v>2</v>
       </c>
@@ -3661,10 +3732,10 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C31" s="83">
         <v>1</v>
@@ -3673,7 +3744,9 @@
         <v>2</v>
       </c>
       <c r="E31" s="85"/>
-      <c r="F31" s="86"/>
+      <c r="F31" s="86">
+        <v>1</v>
+      </c>
       <c r="G31" s="87">
         <v>2</v>
       </c>
@@ -3688,10 +3761,10 @@
     </row>
     <row r="32" spans="1:17" ht="75">
       <c r="A32" s="24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C32" s="83">
         <v>1</v>
@@ -3700,7 +3773,9 @@
         <v>2</v>
       </c>
       <c r="E32" s="85"/>
-      <c r="F32" s="86"/>
+      <c r="F32" s="86">
+        <v>1</v>
+      </c>
       <c r="G32" s="87">
         <v>2</v>
       </c>
@@ -3715,10 +3790,10 @@
     </row>
     <row r="33" spans="1:13" ht="30">
       <c r="A33" s="24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C33" s="83">
         <v>1</v>
@@ -3727,7 +3802,9 @@
         <v>3</v>
       </c>
       <c r="E33" s="85"/>
-      <c r="F33" s="86"/>
+      <c r="F33" s="86">
+        <v>1</v>
+      </c>
       <c r="G33" s="87">
         <v>3</v>
       </c>
@@ -3741,10 +3818,10 @@
       <c r="M33" s="5"/>
     </row>
     <row r="34" spans="1:13" s="44" customFormat="1" ht="15.75">
-      <c r="A34" s="222" t="s">
+      <c r="A34" s="236" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="223"/>
+      <c r="B34" s="237"/>
       <c r="C34" s="47">
         <f>SUMPRODUCT(C30:C33,D30:D33)</f>
         <v>9</v>
@@ -3756,7 +3833,7 @@
       <c r="E34" s="49"/>
       <c r="F34" s="50">
         <f>SUMPRODUCT(F30:F33,G30:G33)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G34" s="51">
         <f>SUM(G30:G33)</f>
@@ -3776,19 +3853,19 @@
       <c r="M34" s="56"/>
     </row>
     <row r="35" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A35" s="229" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" s="229"/>
-      <c r="C35" s="227" t="s">
+      <c r="A35" s="243" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="243"/>
+      <c r="C35" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="228"/>
+      <c r="D35" s="233"/>
       <c r="E35" s="46"/>
-      <c r="F35" s="227" t="s">
+      <c r="F35" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="228"/>
+      <c r="G35" s="233"/>
       <c r="H35" s="46"/>
       <c r="I35" s="68" t="s">
         <v>17</v>
@@ -3800,10 +3877,10 @@
     </row>
     <row r="36" spans="1:13" ht="30">
       <c r="A36" s="29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C36" s="79">
         <v>1</v>
@@ -3812,7 +3889,9 @@
         <v>2</v>
       </c>
       <c r="E36" s="81"/>
-      <c r="F36" s="89"/>
+      <c r="F36" s="89">
+        <v>1</v>
+      </c>
       <c r="G36" s="90">
         <v>2</v>
       </c>
@@ -3827,10 +3906,10 @@
     </row>
     <row r="37" spans="1:13" ht="30">
       <c r="A37" s="23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C37" s="83">
         <v>1</v>
@@ -3839,7 +3918,9 @@
         <v>2</v>
       </c>
       <c r="E37" s="85"/>
-      <c r="F37" s="86"/>
+      <c r="F37" s="86">
+        <v>1</v>
+      </c>
       <c r="G37" s="87">
         <v>2</v>
       </c>
@@ -3854,10 +3935,10 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C38" s="83">
         <v>1</v>
@@ -3866,7 +3947,9 @@
         <v>3</v>
       </c>
       <c r="E38" s="85"/>
-      <c r="F38" s="86"/>
+      <c r="F38" s="86">
+        <v>1</v>
+      </c>
       <c r="G38" s="87">
         <v>3</v>
       </c>
@@ -3881,10 +3964,10 @@
     </row>
     <row r="39" spans="1:13" ht="70.5" customHeight="1">
       <c r="A39" s="23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C39" s="83">
         <v>0.8</v>
@@ -3893,13 +3976,17 @@
         <v>3</v>
       </c>
       <c r="E39" s="85" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" s="86"/>
+        <v>75</v>
+      </c>
+      <c r="F39" s="86">
+        <v>0</v>
+      </c>
       <c r="G39" s="87">
         <v>3</v>
       </c>
-      <c r="H39" s="88"/>
+      <c r="H39" s="88" t="s">
+        <v>76</v>
+      </c>
       <c r="I39" s="76"/>
       <c r="J39" s="77">
         <v>3</v>
@@ -3909,10 +3996,10 @@
       <c r="M39" s="5"/>
     </row>
     <row r="40" spans="1:13" s="44" customFormat="1" ht="15.75">
-      <c r="A40" s="222" t="s">
+      <c r="A40" s="236" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="223"/>
+      <c r="B40" s="237"/>
       <c r="C40" s="69">
         <f>SUMPRODUCT(C36:C39,D36:D39)</f>
         <v>9.4</v>
@@ -3924,7 +4011,7 @@
       <c r="E40" s="49"/>
       <c r="F40" s="70">
         <f>SUMPRODUCT(F36:F39,G36:G39)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G40" s="51">
         <f>SUM(G36:G39)</f>
@@ -3945,35 +4032,37 @@
     </row>
     <row r="41" spans="1:13" ht="18.75" customHeight="1">
       <c r="A41" s="45" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B41" s="45"/>
-      <c r="C41" s="227" t="s">
+      <c r="C41" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="228"/>
+      <c r="D41" s="233"/>
       <c r="E41" s="66" t="s">
-        <v>75</v>
-      </c>
-      <c r="F41" s="227" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="228"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="227" t="s">
+      <c r="G41" s="233"/>
+      <c r="H41" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="I41" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="J41" s="228"/>
+      <c r="J41" s="233"/>
       <c r="K41" s="46"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="1:13" ht="60">
       <c r="A42" s="23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C42" s="83">
         <v>0.75</v>
@@ -3982,9 +4071,11 @@
         <v>2</v>
       </c>
       <c r="E42" s="85" t="s">
-        <v>78</v>
-      </c>
-      <c r="F42" s="86"/>
+        <v>81</v>
+      </c>
+      <c r="F42" s="86">
+        <v>1</v>
+      </c>
       <c r="G42" s="87">
         <v>2</v>
       </c>
@@ -3999,10 +4090,10 @@
     </row>
     <row r="43" spans="1:13" ht="30">
       <c r="A43" s="23" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C43" s="83">
         <v>0.5</v>
@@ -4011,9 +4102,11 @@
         <v>2</v>
       </c>
       <c r="E43" s="85" t="s">
-        <v>81</v>
-      </c>
-      <c r="F43" s="86"/>
+        <v>84</v>
+      </c>
+      <c r="F43" s="86">
+        <v>1</v>
+      </c>
       <c r="G43" s="87">
         <v>2</v>
       </c>
@@ -4028,10 +4121,10 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C44" s="83">
         <v>1</v>
@@ -4040,7 +4133,9 @@
         <v>2</v>
       </c>
       <c r="E44" s="85"/>
-      <c r="F44" s="86"/>
+      <c r="F44" s="86">
+        <v>1</v>
+      </c>
       <c r="G44" s="87">
         <v>2</v>
       </c>
@@ -4052,12 +4147,12 @@
       <c r="K44" s="78"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" ht="45">
       <c r="A45" s="23" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C45" s="83">
         <v>1</v>
@@ -4066,11 +4161,15 @@
         <v>4</v>
       </c>
       <c r="E45" s="85"/>
-      <c r="F45" s="86"/>
+      <c r="F45" s="86">
+        <v>0.75</v>
+      </c>
       <c r="G45" s="87">
         <v>4</v>
       </c>
-      <c r="H45" s="88"/>
+      <c r="H45" s="88" t="s">
+        <v>89</v>
+      </c>
       <c r="I45" s="76"/>
       <c r="J45" s="77">
         <v>4</v>
@@ -4081,10 +4180,10 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C46" s="83">
         <v>1</v>
@@ -4093,7 +4192,9 @@
         <v>6</v>
       </c>
       <c r="E46" s="85"/>
-      <c r="F46" s="86"/>
+      <c r="F46" s="86">
+        <v>1</v>
+      </c>
       <c r="G46" s="87">
         <v>6</v>
       </c>
@@ -4106,12 +4207,12 @@
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
     </row>
-    <row r="47" spans="1:13" ht="45">
+    <row r="47" spans="1:13" ht="120">
       <c r="A47" s="23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C47" s="83">
         <v>0.5</v>
@@ -4120,13 +4221,17 @@
         <v>10</v>
       </c>
       <c r="E47" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="F47" s="86"/>
+        <v>94</v>
+      </c>
+      <c r="F47" s="86">
+        <v>0.5</v>
+      </c>
       <c r="G47" s="87">
         <v>10</v>
       </c>
-      <c r="H47" s="88"/>
+      <c r="H47" s="88" t="s">
+        <v>95</v>
+      </c>
       <c r="I47" s="76"/>
       <c r="J47" s="77">
         <v>10</v>
@@ -4137,10 +4242,10 @@
     </row>
     <row r="48" spans="1:13" ht="30">
       <c r="A48" s="23" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C48" s="83">
         <v>0.85</v>
@@ -4149,13 +4254,17 @@
         <v>6</v>
       </c>
       <c r="E48" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="F48" s="86"/>
+        <v>98</v>
+      </c>
+      <c r="F48" s="86">
+        <v>0.75</v>
+      </c>
       <c r="G48" s="87">
         <v>6</v>
       </c>
-      <c r="H48" s="88"/>
+      <c r="H48" s="88" t="s">
+        <v>99</v>
+      </c>
       <c r="I48" s="76"/>
       <c r="J48" s="77">
         <v>6</v>
@@ -4166,10 +4275,10 @@
     </row>
     <row r="49" spans="1:17">
       <c r="A49" s="13" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C49" s="83">
         <v>1</v>
@@ -4178,7 +4287,9 @@
         <v>3</v>
       </c>
       <c r="E49" s="85"/>
-      <c r="F49" s="86"/>
+      <c r="F49" s="86">
+        <v>1</v>
+      </c>
       <c r="G49" s="87">
         <v>3</v>
       </c>
@@ -4192,10 +4303,10 @@
       <c r="M49" s="5"/>
     </row>
     <row r="50" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A50" s="222" t="s">
+      <c r="A50" s="236" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="223"/>
+      <c r="B50" s="237"/>
       <c r="C50" s="71">
         <f>SUMPRODUCT(C42:C49,D42:D49)</f>
         <v>27.6</v>
@@ -4207,7 +4318,7 @@
       <c r="E50" s="59"/>
       <c r="F50" s="70">
         <f>SUMPRODUCT(F42:F49,G42:G49)</f>
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="G50" s="51">
         <f>SUM(G42:G49)</f>
@@ -4231,34 +4342,34 @@
       <c r="Q50" s="44"/>
     </row>
     <row r="51" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A51" s="229" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="229"/>
-      <c r="C51" s="227" t="s">
+      <c r="A51" s="243" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="243"/>
+      <c r="C51" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="228"/>
+      <c r="D51" s="233"/>
       <c r="E51" s="46"/>
-      <c r="F51" s="227" t="s">
+      <c r="F51" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="G51" s="228"/>
+      <c r="G51" s="233"/>
       <c r="H51" s="46"/>
-      <c r="I51" s="227" t="s">
+      <c r="I51" s="232" t="s">
         <v>17</v>
       </c>
-      <c r="J51" s="228"/>
+      <c r="J51" s="233"/>
       <c r="K51" s="46"/>
       <c r="L51" s="8"/>
       <c r="M51" s="4"/>
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="29" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C52" s="79">
         <v>1</v>
@@ -4267,7 +4378,9 @@
         <v>2</v>
       </c>
       <c r="E52" s="81"/>
-      <c r="F52" s="82"/>
+      <c r="F52" s="82">
+        <v>1</v>
+      </c>
       <c r="G52" s="27">
         <v>2</v>
       </c>
@@ -4282,10 +4395,10 @@
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="23" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C53" s="83">
         <v>1</v>
@@ -4294,7 +4407,9 @@
         <v>2</v>
       </c>
       <c r="E53" s="85"/>
-      <c r="F53" s="86"/>
+      <c r="F53" s="86">
+        <v>1</v>
+      </c>
       <c r="G53" s="87">
         <v>2</v>
       </c>
@@ -4309,10 +4424,10 @@
     </row>
     <row r="54" spans="1:17" ht="30">
       <c r="A54" s="23" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C54" s="83">
         <v>1</v>
@@ -4321,7 +4436,9 @@
         <v>1</v>
       </c>
       <c r="E54" s="85"/>
-      <c r="F54" s="86"/>
+      <c r="F54" s="86">
+        <v>1</v>
+      </c>
       <c r="G54" s="87">
         <v>1</v>
       </c>
@@ -4336,10 +4453,10 @@
     </row>
     <row r="55" spans="1:17" ht="60">
       <c r="A55" s="23" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C55" s="83">
         <v>1</v>
@@ -4348,7 +4465,9 @@
         <v>4</v>
       </c>
       <c r="E55" s="85"/>
-      <c r="F55" s="86"/>
+      <c r="F55" s="86">
+        <v>1</v>
+      </c>
       <c r="G55" s="87">
         <v>4</v>
       </c>
@@ -4363,10 +4482,10 @@
     </row>
     <row r="56" spans="1:17" ht="30">
       <c r="A56" s="23" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C56" s="83">
         <v>1</v>
@@ -4375,7 +4494,9 @@
         <v>2</v>
       </c>
       <c r="E56" s="85"/>
-      <c r="F56" s="86"/>
+      <c r="F56" s="86">
+        <v>1</v>
+      </c>
       <c r="G56" s="87">
         <v>2</v>
       </c>
@@ -4389,10 +4510,10 @@
       <c r="M56" s="5"/>
     </row>
     <row r="57" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A57" s="222" t="s">
+      <c r="A57" s="236" t="s">
         <v>25</v>
       </c>
-      <c r="B57" s="223"/>
+      <c r="B57" s="237"/>
       <c r="C57" s="57">
         <f>SUMPRODUCT(C52:C56,D52:D56)</f>
         <v>11</v>
@@ -4404,7 +4525,7 @@
       <c r="E57" s="59"/>
       <c r="F57" s="60">
         <f>SUMPRODUCT(F52:F56,G52:G56)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G57" s="61">
         <f>SUM(G52:G56)</f>
@@ -4424,27 +4545,27 @@
       <c r="M57" s="56"/>
     </row>
     <row r="58" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A58" s="224" t="s">
+      <c r="A58" s="266" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="225"/>
-      <c r="C58" s="225"/>
-      <c r="D58" s="225"/>
-      <c r="E58" s="225"/>
-      <c r="F58" s="225"/>
-      <c r="G58" s="225"/>
-      <c r="H58" s="225"/>
-      <c r="I58" s="225"/>
-      <c r="J58" s="225"/>
-      <c r="K58" s="226"/>
+      <c r="B58" s="267"/>
+      <c r="C58" s="267"/>
+      <c r="D58" s="267"/>
+      <c r="E58" s="267"/>
+      <c r="F58" s="267"/>
+      <c r="G58" s="267"/>
+      <c r="H58" s="267"/>
+      <c r="I58" s="267"/>
+      <c r="J58" s="267"/>
+      <c r="K58" s="268"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
     </row>
     <row r="59" spans="1:17">
-      <c r="A59" s="230" t="s">
-        <v>107</v>
-      </c>
-      <c r="B59" s="231"/>
+      <c r="A59" s="253" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="254"/>
       <c r="C59" s="34">
         <f>C18+C23+C28+C34+C40+C50+C57+C11</f>
         <v>79.650000000000006</v>
@@ -4456,7 +4577,7 @@
       <c r="E59" s="26"/>
       <c r="F59" s="35">
         <f>F18+F23+F28+F34+F40+F50+F57+F11</f>
-        <v>0</v>
+        <v>85.5</v>
       </c>
       <c r="G59" s="27">
         <f>G11+G18+G23+G28+G34+G40+G50+G57</f>
@@ -4476,33 +4597,69 @@
       <c r="M59" s="5"/>
     </row>
     <row r="60" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A60" s="232" t="s">
-        <v>108</v>
-      </c>
-      <c r="B60" s="233"/>
-      <c r="C60" s="234">
+      <c r="A60" s="255" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" s="256"/>
+      <c r="C60" s="257">
         <f>C59/D59</f>
         <v>0.7965000000000001</v>
       </c>
-      <c r="D60" s="235"/>
-      <c r="E60" s="236"/>
-      <c r="F60" s="237">
+      <c r="D60" s="258"/>
+      <c r="E60" s="259"/>
+      <c r="F60" s="260">
         <f>F59/G59</f>
-        <v>0</v>
-      </c>
-      <c r="G60" s="238"/>
-      <c r="H60" s="239"/>
-      <c r="I60" s="240">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="G60" s="261"/>
+      <c r="H60" s="262"/>
+      <c r="I60" s="263">
         <f>I59/J59</f>
         <v>0</v>
       </c>
-      <c r="J60" s="241"/>
-      <c r="K60" s="242"/>
+      <c r="J60" s="264"/>
+      <c r="K60" s="265"/>
       <c r="L60" s="72"/>
       <c r="M60" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="I60:K60"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F35:G35"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="I6:K6"/>
@@ -4519,42 +4676,6 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="I60:K60"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L18 L23 L28 L34 L40 L50 L11 C9:C10 F9:F10 I9:I10 C13:C17 F13:F17 I13:I17 C20:C22 F20:F22 I20:I22 C25:C27 F25:F27 I25:I27 C30:C33 F30:F33 I30:I33 C36:C39 F36:F39 I36:I39 C42:C49 F42:F49 I42:I49 C52:C56 F52:F56 I52:I56" xr:uid="{4A0D4DC8-F6F9-4765-AB49-E4E0ACDB1361}">
@@ -4576,8 +4697,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4592,15 +4713,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="266" t="s">
+      <c r="A2" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="266"/>
-      <c r="E2" s="266"/>
-      <c r="F2" s="266"/>
-      <c r="G2" s="266"/>
+      <c r="B2" s="269"/>
+      <c r="C2" s="269"/>
+      <c r="D2" s="269"/>
+      <c r="E2" s="269"/>
+      <c r="F2" s="269"/>
+      <c r="G2" s="269"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="38"/>
@@ -4613,7 +4734,7 @@
     </row>
     <row r="4" spans="1:7" ht="18.75">
       <c r="A4" s="36" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -4624,31 +4745,31 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:7" ht="23.25">
-      <c r="A6" s="270" t="s">
+      <c r="A6" s="273" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="271"/>
-      <c r="C6" s="271"/>
-      <c r="D6" s="271"/>
-      <c r="E6" s="271"/>
-      <c r="F6" s="271"/>
-      <c r="G6" s="272"/>
+      <c r="B6" s="274"/>
+      <c r="C6" s="274"/>
+      <c r="D6" s="274"/>
+      <c r="E6" s="274"/>
+      <c r="F6" s="274"/>
+      <c r="G6" s="275"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="130" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B7" s="131" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="131" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D7" s="131" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="131" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F7" s="131" t="s">
         <v>17</v>
@@ -4659,7 +4780,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="133" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B8" s="134">
         <v>1</v>
@@ -4679,7 +4800,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="136" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B9" s="137">
         <v>0.9</v>
@@ -4696,12 +4817,12 @@
       </c>
       <c r="F9" s="137"/>
       <c r="G9" s="138" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45">
       <c r="A10" s="133" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B10" s="134">
         <v>0.9</v>
@@ -4717,13 +4838,13 @@
         <v>18</v>
       </c>
       <c r="F10" s="134"/>
-      <c r="G10" s="277" t="s">
-        <v>117</v>
+      <c r="G10" s="222" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="136" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B11" s="137">
         <v>0.9</v>
@@ -4740,12 +4861,12 @@
       </c>
       <c r="F11" s="137"/>
       <c r="G11" s="138" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="133" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B12" s="134">
         <v>1</v>
@@ -4765,7 +4886,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="133" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B13" s="134">
         <v>1</v>
@@ -4785,7 +4906,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="136" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B14" s="137">
         <v>1</v>
@@ -4805,7 +4926,7 @@
     </row>
     <row r="15" spans="1:7" ht="30">
       <c r="A15" s="133" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B15" s="134">
         <v>0.95</v>
@@ -4821,13 +4942,13 @@
         <v>9.5</v>
       </c>
       <c r="F15" s="134"/>
-      <c r="G15" s="278" t="s">
-        <v>124</v>
+      <c r="G15" s="223" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="136" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B16" s="137">
         <v>1</v>
@@ -4847,7 +4968,7 @@
     </row>
     <row r="17" spans="1:7" ht="30">
       <c r="A17" s="139" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B17" s="140">
         <v>0.9</v>
@@ -4863,16 +4984,16 @@
         <v>5.4</v>
       </c>
       <c r="F17" s="140"/>
-      <c r="G17" s="279" t="s">
-        <v>127</v>
+      <c r="G17" s="224" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="141" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="273"/>
-      <c r="C18" s="273"/>
+        <v>134</v>
+      </c>
+      <c r="B18" s="276"/>
+      <c r="C18" s="276"/>
       <c r="D18" s="142">
         <f>SUM(D8:D17)</f>
         <v>100</v>
@@ -4886,7 +5007,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="145" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B19" s="146" t="s">
         <v>14</v>
@@ -4896,7 +5017,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="147" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F19" s="147"/>
       <c r="G19" s="148" t="s">
@@ -4905,7 +5026,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="149" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B20" s="150">
         <v>0.3</v>
@@ -4920,12 +5041,12 @@
       </c>
       <c r="F20" s="150"/>
       <c r="G20" s="152" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="153" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B21" s="154">
         <v>0</v>
@@ -4942,31 +5063,31 @@
       <c r="G21" s="156"/>
     </row>
     <row r="22" spans="1:7" ht="23.25">
-      <c r="A22" s="274" t="s">
+      <c r="A22" s="277" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="275"/>
-      <c r="C22" s="275"/>
-      <c r="D22" s="275"/>
-      <c r="E22" s="275"/>
-      <c r="F22" s="275"/>
-      <c r="G22" s="276"/>
+      <c r="B22" s="278"/>
+      <c r="C22" s="278"/>
+      <c r="D22" s="278"/>
+      <c r="E22" s="278"/>
+      <c r="F22" s="278"/>
+      <c r="G22" s="279"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="157" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B23" s="158" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="158" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D23" s="158" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="158" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F23" s="158" t="s">
         <v>17</v>
@@ -4977,207 +5098,211 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="160" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B24" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="161">
         <v>20</v>
       </c>
       <c r="E24" s="161">
         <f>B24*C24*D24</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F24" s="161"/>
       <c r="G24" s="162"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="163" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B25" s="164">
-        <v>0</v>
-      </c>
-      <c r="C25" s="164">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C25" s="161">
+        <v>1</v>
       </c>
       <c r="D25" s="164">
         <v>6</v>
       </c>
       <c r="E25" s="164">
         <f t="shared" ref="E25:E33" si="1">B25*C25*D25</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F25" s="164"/>
       <c r="G25" s="165"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="160" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B26" s="161">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="C26" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="161">
         <v>12</v>
       </c>
       <c r="E26" s="161">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11.399999999999999</v>
       </c>
       <c r="F26" s="161"/>
-      <c r="G26" s="162"/>
+      <c r="G26" s="162" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="163" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B27" s="164">
-        <v>0</v>
-      </c>
-      <c r="C27" s="164">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="161">
+        <v>1</v>
       </c>
       <c r="D27" s="164">
         <v>8</v>
       </c>
       <c r="E27" s="164">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F27" s="164"/>
       <c r="G27" s="165"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="160" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B28" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="161">
         <v>6</v>
       </c>
       <c r="E28" s="161">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F28" s="161"/>
       <c r="G28" s="162"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="163" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B29" s="164">
-        <v>0</v>
-      </c>
-      <c r="C29" s="164">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C29" s="161">
+        <v>1</v>
       </c>
       <c r="D29" s="164">
         <v>14</v>
       </c>
       <c r="E29" s="164">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F29" s="164"/>
       <c r="G29" s="165"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="160" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B30" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="161">
         <v>12</v>
       </c>
       <c r="E30" s="161">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F30" s="161"/>
       <c r="G30" s="162"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="163" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B31" s="164">
-        <v>0</v>
-      </c>
-      <c r="C31" s="164">
-        <v>0</v>
+        <v>0.95</v>
+      </c>
+      <c r="C31" s="161">
+        <v>1</v>
       </c>
       <c r="D31" s="164">
         <v>4</v>
       </c>
       <c r="E31" s="164">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F31" s="164"/>
-      <c r="G31" s="165"/>
+      <c r="G31" s="165" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="160" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B32" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="161">
         <v>10</v>
       </c>
       <c r="E32" s="161">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F32" s="161"/>
       <c r="G32" s="162"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="166" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B33" s="167">
-        <v>0</v>
-      </c>
-      <c r="C33" s="167">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C33" s="161">
+        <v>1</v>
       </c>
       <c r="D33" s="167">
         <v>8</v>
       </c>
       <c r="E33" s="167">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F33" s="167"/>
       <c r="G33" s="168"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="169" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B34" s="170"/>
       <c r="C34" s="170"/>
@@ -5187,14 +5312,14 @@
       </c>
       <c r="E34" s="171">
         <f>(SUM(E24:E33) + E36+E37+E38)/D34</f>
-        <v>0</v>
+        <v>0.96700000000000008</v>
       </c>
       <c r="F34" s="171"/>
       <c r="G34" s="172"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="173" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B35" s="174" t="s">
         <v>14</v>
@@ -5204,7 +5329,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="175" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F35" s="175"/>
       <c r="G35" s="176" t="s">
@@ -5213,10 +5338,10 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="177" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B36" s="178">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C36" s="178"/>
       <c r="D36" s="179">
@@ -5224,14 +5349,16 @@
       </c>
       <c r="E36" s="178">
         <f>B36*D36</f>
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="F36" s="178"/>
-      <c r="G36" s="180"/>
+      <c r="G36" s="180" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="181" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B37" s="182">
         <v>0</v>
@@ -5249,7 +5376,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="185" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B38" s="186">
         <v>0</v>
@@ -5266,31 +5393,31 @@
       <c r="G38" s="188"/>
     </row>
     <row r="39" spans="1:7" ht="23.25">
-      <c r="A39" s="267" t="s">
+      <c r="A39" s="270" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="268"/>
-      <c r="C39" s="268"/>
-      <c r="D39" s="268"/>
-      <c r="E39" s="268"/>
-      <c r="F39" s="268"/>
-      <c r="G39" s="269"/>
+      <c r="B39" s="271"/>
+      <c r="C39" s="271"/>
+      <c r="D39" s="271"/>
+      <c r="E39" s="271"/>
+      <c r="F39" s="271"/>
+      <c r="G39" s="272"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="189" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B40" s="190" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="190" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D40" s="190" t="s">
         <v>4</v>
       </c>
       <c r="E40" s="190" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F40" s="190" t="s">
         <v>17</v>
@@ -5301,7 +5428,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="192" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B41" s="193">
         <v>0</v>
@@ -5321,7 +5448,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="195" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B42" s="196">
         <v>0</v>
@@ -5341,7 +5468,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="192" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="B43" s="193">
         <v>0</v>
@@ -5361,7 +5488,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="195" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="B44" s="196">
         <v>0</v>
@@ -5381,7 +5508,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="192" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B45" s="193">
         <v>0</v>
@@ -5401,7 +5528,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="195" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B46" s="196">
         <v>0</v>
@@ -5421,7 +5548,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="192" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B47" s="193">
         <v>0</v>
@@ -5441,7 +5568,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="195" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B48" s="196">
         <v>0</v>
@@ -5461,7 +5588,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="198" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B49" s="199">
         <v>0</v>
@@ -5481,7 +5608,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="201" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B50" s="202"/>
       <c r="C50" s="202"/>
@@ -5498,7 +5625,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="205" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B51" s="206" t="s">
         <v>14</v>
@@ -5508,7 +5635,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="207" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F51" s="207"/>
       <c r="G51" s="208" t="s">
@@ -5517,7 +5644,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="209" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B52" s="210">
         <v>0</v>
@@ -5535,7 +5662,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="213" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B53" s="214">
         <v>0</v>
@@ -5553,7 +5680,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="217" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B54" s="218">
         <v>0</v>
@@ -5596,12 +5723,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B41E0342602C49449CD93109DBCAB8C5" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4cab946e3812a26735e8b0dc00d59aca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3ea4e87-b30d-4ccc-9564-7710f23c54f0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afa808ced5dc9827eedaaa69eb8b35dd" ns2:_="">
     <xsd:import namespace="d3ea4e87-b30d-4ccc-9564-7710f23c54f0"/>
@@ -5733,6 +5854,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5743,11 +5870,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1971BE-1E76-44E5-BF52-2DB1BB889C58}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1971BE-1E76-44E5-BF52-2DB1BB889C58}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>